<commit_message>
Updated with latest and added tribunal office information from postDefaultValues
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">FIELDS</t>
   </si>
@@ -32,6 +32,48 @@
   </si>
   <si>
     <t xml:space="preserve">Awaiting ET3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35 La Nava S3 6AD, Southampton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterTelephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterFax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manchester@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalGlasgowAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35 High Landing G3 6AD, Glasgow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalGlasgowTelephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalGlasgowFax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalGlasgowDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalGlasgowEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">glasgow@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -115,7 +157,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -132,6 +174,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,16 +195,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.28"/>
@@ -187,9 +233,91 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3577131270</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>7577126570</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3572531270</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2937126570</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1231123</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" display="manchester@gmail.com"/>
+    <hyperlink ref="B12" r:id="rId2" display="glasgow@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
ERP-347 - As a Case Work Clerk I want the venue details to be populated on any correspondence documents that are created
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">FIELDS</t>
   </si>
@@ -37,43 +37,61 @@
     <t xml:space="preserve">tribunalManchesterAddress</t>
   </si>
   <si>
-    <t xml:space="preserve">35 La Nava S3 6AD, Southampton</t>
+    <t xml:space="preserve">Manchester Employment Tribunal, Alexandra House, 14-22 The Parsonage, Manchester, M3 2JA</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalManchesterTelephone</t>
   </si>
   <si>
+    <t xml:space="preserve">0161 833 6100</t>
+  </si>
+  <si>
     <t xml:space="preserve">tribunalManchesterFax</t>
   </si>
   <si>
+    <t xml:space="preserve">0870 739 4433</t>
+  </si>
+  <si>
     <t xml:space="preserve">tribunalManchesterDX</t>
   </si>
   <si>
+    <t xml:space="preserve">DX 743570</t>
+  </si>
+  <si>
     <t xml:space="preserve">tribunalManchesterEmail</t>
   </si>
   <si>
-    <t xml:space="preserve">manchester@gmail.com</t>
+    <t xml:space="preserve">Manchesteret@justice.gov.uk</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalGlasgowAddress</t>
   </si>
   <si>
-    <t xml:space="preserve">35 High Landing G3 6AD, Glasgow</t>
+    <t xml:space="preserve">Eagle Building, 215 Bothwell Street, Glasgow, G2 7TS</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalGlasgowTelephone</t>
   </si>
   <si>
+    <t xml:space="preserve">0141 204 0730</t>
+  </si>
+  <si>
     <t xml:space="preserve">tribunalGlasgowFax</t>
   </si>
   <si>
+    <t xml:space="preserve">01264 785 177</t>
+  </si>
+  <si>
     <t xml:space="preserve">tribunalGlasgowDX</t>
   </si>
   <si>
+    <t xml:space="preserve">DX 7435701</t>
+  </si>
+  <si>
     <t xml:space="preserve">tribunalGlasgowEmail</t>
   </si>
   <si>
-    <t xml:space="preserve">glasgow@gmail.com</t>
+    <t xml:space="preserve">glasgowet@justice.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -245,78 +263,78 @@
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>3577131270</v>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>7577126570</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>123456</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>3572531270</v>
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>2937126570</v>
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>1231123</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="manchester@gmail.com"/>
-    <hyperlink ref="B12" r:id="rId2" display="glasgow@gmail.com"/>
+    <hyperlink ref="B7" r:id="rId1" display="Manchesteret@justice.gov.uk"/>
+    <hyperlink ref="B12" r:id="rId2" display="glasgowet@justice.gov.uk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
ERP-435 - As a Case Work Clerk I want the address to be separated onto multiple lines when generating letters
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t xml:space="preserve">FIELDS</t>
   </si>
@@ -34,10 +34,34 @@
     <t xml:space="preserve">Awaiting ET3</t>
   </si>
   <si>
-    <t xml:space="preserve">tribunalManchesterAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manchester Employment Tribunal, Alexandra House, 14-22 The Parsonage, Manchester, M3 2JA</t>
+    <t xml:space="preserve">tribunalManchesterAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester Employment Tribunal,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alexandra House,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterAddressLine3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14-22 The Parsonage,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manchester,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalManchesterPostCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M3 2JA</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalManchesterTelephone</t>
@@ -64,10 +88,28 @@
     <t xml:space="preserve">Manchesteret@justice.gov.uk</t>
   </si>
   <si>
-    <t xml:space="preserve">tribunalGlasgowAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eagle Building, 215 Bothwell Street, Glasgow, G2 7TS</t>
+    <t xml:space="preserve">tribunalGlasgowAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eagle Building,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalGlasgowAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">215 Bothwell Street,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalGlasgowTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glasgow,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalGlasgowPostCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G2 7TS</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalGlasgowTelephone</t>
@@ -101,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -132,6 +174,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -175,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +244,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,10 +265,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -251,51 +303,55 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="H3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -327,14 +383,70 @@
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="4" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="Manchesteret@justice.gov.uk"/>
-    <hyperlink ref="B12" r:id="rId2" display="glasgowet@justice.gov.uk"/>
+    <hyperlink ref="B11" r:id="rId1" display="Manchesteret@justice.gov.uk"/>
+    <hyperlink ref="B19" r:id="rId2" display="glasgowet@justice.gov.uk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
ERP-444 - Add a new current position for manual creation
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">positionType</t>
   </si>
   <si>
-    <t xml:space="preserve">Awaiting ET3</t>
+    <t xml:space="preserve">Manually Created</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalManchesterAddressLine1</t>
@@ -143,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -174,12 +174,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,7 +217,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,10 +238,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -268,7 +258,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -399,7 +389,7 @@
       <c r="A14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ERP-483 - As a Case Worker I want the managing office to be defaulted to Glasgow when creating a case
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">FIELDS</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t xml:space="preserve">glasgowet@justice.gov.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">managingOffice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Glasgow</t>
   </si>
 </sst>
 </file>
@@ -255,10 +261,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -431,6 +437,14 @@
       </c>
       <c r="B19" s="0" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ERP-514 - Remove , from the court address
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t xml:space="preserve">FIELDS</t>
   </si>
@@ -37,25 +37,25 @@
     <t xml:space="preserve">tribunalManchesterAddressLine1</t>
   </si>
   <si>
-    <t xml:space="preserve">Manchester Employment Tribunal,</t>
+    <t xml:space="preserve">Manchester Employment Tribunal</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalManchesterAddressLine2</t>
   </si>
   <si>
-    <t xml:space="preserve">Alexandra House,</t>
+    <t xml:space="preserve">Alexandra House</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalManchesterAddressLine3</t>
   </si>
   <si>
-    <t xml:space="preserve">14-22 The Parsonage,</t>
+    <t xml:space="preserve">14-22 The Parsonage</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalManchesterTown</t>
   </si>
   <si>
-    <t xml:space="preserve">Manchester,</t>
+    <t xml:space="preserve">Manchester</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalManchesterPostCode</t>
@@ -91,19 +91,19 @@
     <t xml:space="preserve">tribunalGlasgowAddressLine1</t>
   </si>
   <si>
-    <t xml:space="preserve">Eagle Building,</t>
+    <t xml:space="preserve">Eagle Building</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalGlasgowAddressLine2</t>
   </si>
   <si>
-    <t xml:space="preserve">215 Bothwell Street,</t>
+    <t xml:space="preserve">215 Bothwell Street</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalGlasgowTown</t>
   </si>
   <si>
-    <t xml:space="preserve">Glasgow,</t>
+    <t xml:space="preserve">Glasgow</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalGlasgowPostCode</t>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t xml:space="preserve">managingOffice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Glasgow</t>
   </si>
 </sst>
 </file>
@@ -264,7 +261,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -444,7 +441,7 @@
         <v>38</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ERP-521 - As a Case Work Clerk I want the outstation address to appear on letters generated for Scottish outstations
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
   <si>
     <t xml:space="preserve">FIELDS</t>
   </si>
@@ -137,6 +137,147 @@
   </si>
   <si>
     <t xml:space="preserve">managingOffice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalAberdeenAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ground Floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalAberdeenAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB1, 48 Huntly Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalAberdeenTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aberdeen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalAberdeenPostCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AB10 1SH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalAberdeenTelephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01224 593 137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalAberdeenFax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0870 761 7766</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalAberdeenDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DX AB77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalAberdeenEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aberdeenet@justice.gov.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeeAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeeAddressLine2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Block C, Caledonian House</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeeAddressLine3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greenmarket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeeTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dundee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeePostCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DD1 4QG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeeTelephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01382 221 578</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeeFax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01382 227 136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeeDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DX DD51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalDundeeEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dundeeet@justice.gov.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalEdinburghAddressLine1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54-56 Melville Street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalEdinburghTown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edinburgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalEdinburghPostCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EH3 7HF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalEdinburghTelephone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0131 226 5584</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalEdinburghFax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0131 220 6847</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalEdinburghDX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DX ED147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tribunalEdinburghEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">edinburghet@justice.gov.uk</t>
   </si>
 </sst>
 </file>
@@ -258,10 +399,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -444,10 +585,205 @@
         <v>27</v>
       </c>
     </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" display="Manchesteret@justice.gov.uk"/>
     <hyperlink ref="B19" r:id="rId2" display="glasgowet@justice.gov.uk"/>
+    <hyperlink ref="B28" r:id="rId3" display="aberdeenet@justice.gov.uk"/>
+    <hyperlink ref="B37" r:id="rId4" display="dundeeet@justice.gov.uk"/>
+    <hyperlink ref="B44" r:id="rId5" display="edinburghet@justice.gov.uk"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Respondent Address and Single Value
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="248">
   <si>
     <t xml:space="preserve">FIELDS</t>
   </si>
@@ -758,6 +758,12 @@
   </si>
   <si>
     <t xml:space="preserve">watfordet@justice.gov.uk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caseType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
   </si>
 </sst>
 </file>
@@ -881,8 +887,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1911,6 +1917,14 @@
       </c>
       <c r="B126" s="0" t="s">
         <v>245</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="B127" s="0" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
ERP-797 - LEEDS - Update Leeds Tribunal contact details (Fax machine number and email address)
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -367,13 +367,13 @@
     <t xml:space="preserve">tribunalLeedsFax</t>
   </si>
   <si>
-    <t xml:space="preserve">0113 242 8843</t>
+    <t xml:space="preserve">01264 785136</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalLeedsEmail</t>
   </si>
   <si>
-    <t xml:space="preserve">leedset@hmcts.gsi.gov.uk</t>
+    <t xml:space="preserve">LeedsET@justice.gov.uk</t>
   </si>
   <si>
     <t xml:space="preserve">tribunalLondonCentralAddressLine1</t>
@@ -887,8 +887,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A108" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A127" activeCellId="0" sqref="A127"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B60" activeCellId="0" sqref="A59:B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1953,7 +1953,7 @@
     <hyperlink ref="B37" r:id="rId4" display="dundeeet@justice.gov.uk"/>
     <hyperlink ref="B44" r:id="rId5" display="edinburghet@justice.gov.uk"/>
     <hyperlink ref="B52" r:id="rId6" display="bristolet@justice.gov.uk"/>
-    <hyperlink ref="B60" r:id="rId7" display="leedset@hmcts.gsi.gov.uk"/>
+    <hyperlink ref="B60" r:id="rId7" display="LeedsET@justice.gov.uk"/>
     <hyperlink ref="B69" r:id="rId8" display="londoncentralet@hmcts.gsi.gov.uk"/>
     <hyperlink ref="B77" r:id="rId9" display="eastlondon@justice.gov.uk"/>
     <hyperlink ref="B86" r:id="rId10" display="londonsouthet@hmcts.gsi.gov.uk"/>

</xml_diff>

<commit_message>
Updated glasgow tribunal office
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rabab/HMCTS/ethos-repl-docmosis-service/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andcolli\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499608D1-C828-E04D-A5B5-6E5A00D38843}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6BBE4B5-E89E-4583-AC0F-097BF4F3A32C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26480" windowHeight="16260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-6930" windowWidth="21840" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="251">
   <si>
     <t>FIELDS</t>
   </si>
@@ -96,15 +96,9 @@
     <t>tribunalGlasgowAddressLine1</t>
   </si>
   <si>
-    <t>Eagle Building</t>
-  </si>
-  <si>
     <t>tribunalGlasgowAddressLine2</t>
   </si>
   <si>
-    <t>215 Bothwell Street</t>
-  </si>
-  <si>
     <t>tribunalGlasgowTown</t>
   </si>
   <si>
@@ -114,9 +108,6 @@
     <t>tribunalGlasgowPostCode</t>
   </si>
   <si>
-    <t>G2 7TS</t>
-  </si>
-  <si>
     <t>tribunalGlasgowTelephone</t>
   </si>
   <si>
@@ -772,6 +763,21 @@
   </si>
   <si>
     <t>01264 887 302</t>
+  </si>
+  <si>
+    <t>Glasgow Tribunals Centre</t>
+  </si>
+  <si>
+    <t>3 Atlantic Quay</t>
+  </si>
+  <si>
+    <t>20 York Street</t>
+  </si>
+  <si>
+    <t>tribunalGlasgowAddressLine3</t>
+  </si>
+  <si>
+    <t>G2 8GT</t>
   </si>
 </sst>
 </file>
@@ -1141,26 +1147,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="1025" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="1025" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1169,7 +1175,7 @@
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1178,7 +1184,7 @@
       </c>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1187,7 +1193,7 @@
       </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -1196,7 +1202,7 @@
       </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1205,7 +1211,7 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1214,7 +1220,7 @@
       </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1223,7 +1229,7 @@
       </c>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1239,7 +1245,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1247,7 +1253,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1255,951 +1261,959 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>249</v>
+      </c>
+      <c r="B14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B16" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="B23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="4" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="4" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="B25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="4" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B26" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="4" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B27" t="s">
         <v>47</v>
       </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="B28" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="B29" t="s">
         <v>51</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B30" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>53</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="B32" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="4" t="s">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="B33" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B31" s="4" t="s">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="B34" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="4" t="s">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="B35" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="4" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="B36" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B37" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="B39" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="B40" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="4" t="s">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="B41" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="4" t="s">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="B42" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="4" t="s">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="B43" t="s">
         <v>78</v>
       </c>
-      <c r="B41" t="s">
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="B44" t="s">
         <v>80</v>
       </c>
-      <c r="B42" t="s">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="B45" t="s">
         <v>82</v>
       </c>
-      <c r="B43" t="s">
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B46" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B44" t="s">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="B47" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="4" t="s">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="B48" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B46" s="4" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="B49" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="4" t="s">
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="B50" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="4" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="B51" t="s">
         <v>94</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="B52" t="s">
         <v>96</v>
       </c>
-      <c r="B50" t="s">
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
+      <c r="B53" t="s">
         <v>98</v>
       </c>
-      <c r="B51" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
+      <c r="B54" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B52" t="s">
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
+      <c r="B55" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B53" s="4" t="s">
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
+      <c r="B56" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B54" s="4" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
+      <c r="B57" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="4" t="s">
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
+      <c r="B58" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B56" s="4" t="s">
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
+      <c r="B59" t="s">
         <v>110</v>
       </c>
-      <c r="B57" s="4" t="s">
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
+      <c r="B60" t="s">
         <v>112</v>
       </c>
-      <c r="B58" t="s">
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
+      <c r="B61" t="s">
         <v>114</v>
       </c>
-      <c r="B59" t="s">
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
+      <c r="B62" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>116</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="B64" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="4" t="s">
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="B65" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B63" s="4" t="s">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
+      <c r="B66" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B64" s="4" t="s">
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="B67" t="s">
         <v>125</v>
       </c>
-      <c r="B65" s="4" t="s">
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+      <c r="B68" t="s">
         <v>127</v>
       </c>
-      <c r="B66" t="s">
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
+      <c r="B69" t="s">
         <v>129</v>
       </c>
-      <c r="B67" t="s">
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="B70" t="s">
         <v>131</v>
       </c>
-      <c r="B68" t="s">
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+      <c r="B71" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B69" t="s">
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
+      <c r="B72" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="B70" s="4" t="s">
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
+      <c r="B73" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B71" s="4" t="s">
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="B74" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>139</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B75" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>141</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+      <c r="B76" t="s">
         <v>142</v>
       </c>
-      <c r="B74" s="4" t="s">
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
+      <c r="B77" t="s">
         <v>144</v>
       </c>
-      <c r="B75" t="s">
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="B78" t="s">
         <v>146</v>
       </c>
-      <c r="B76" t="s">
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="B79" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B77" t="s">
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+      <c r="B80" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B78" s="4" t="s">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+      <c r="B81" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B79" s="4" t="s">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
+      <c r="B82" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>154</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>156</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="B84" t="s">
         <v>157</v>
       </c>
-      <c r="B82" s="4" t="s">
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
+      <c r="B85" t="s">
         <v>159</v>
       </c>
-      <c r="B83" t="s">
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
+      <c r="B86" t="s">
         <v>161</v>
       </c>
-      <c r="B84" t="s">
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+      <c r="B87" t="s">
         <v>163</v>
       </c>
-      <c r="B85" t="s">
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+      <c r="B88" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B86" t="s">
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
+      <c r="B89" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="B87" s="4" t="s">
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
+      <c r="B90" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B88" s="4" t="s">
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="B91" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B89" s="4" t="s">
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+      <c r="B92" t="s">
         <v>173</v>
       </c>
-      <c r="B90" s="4" t="s">
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+      <c r="B93" t="s">
         <v>175</v>
       </c>
-      <c r="B91" t="s">
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
+      <c r="B94" t="s">
         <v>177</v>
       </c>
-      <c r="B92" t="s">
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
+      <c r="B95" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B93" t="s">
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
+      <c r="B96" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B94" s="4" t="s">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
+      <c r="B97" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B95" s="4" t="s">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
+      <c r="B98" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="B96" s="4" t="s">
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
+      <c r="B99" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B97" s="4" t="s">
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
+      <c r="B100" t="s">
         <v>189</v>
       </c>
-      <c r="B98" s="4" t="s">
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" t="s">
+      <c r="B101" t="s">
         <v>191</v>
       </c>
-      <c r="B99" t="s">
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="B102" t="s">
         <v>193</v>
       </c>
-      <c r="B100" t="s">
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101" t="s">
+      <c r="B103" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B101" t="s">
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102" t="s">
+      <c r="B104" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B102" s="4" t="s">
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="B105" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B103" s="4" t="s">
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+      <c r="B106" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B104" s="4" t="s">
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
+      <c r="B107" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="B105" s="4" t="s">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
+      <c r="B108" t="s">
         <v>205</v>
       </c>
-      <c r="B106" s="4" t="s">
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" t="s">
+      <c r="B109" t="s">
         <v>207</v>
       </c>
-      <c r="B107" t="s">
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="B110" t="s">
         <v>209</v>
       </c>
-      <c r="B108" t="s">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
+      <c r="B111" t="s">
         <v>211</v>
       </c>
-      <c r="B109" t="s">
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
+      <c r="B112" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B110" t="s">
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111" t="s">
+      <c r="B113" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="B111" s="4" t="s">
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="B114" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="B112" s="4" t="s">
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
+      <c r="B115" t="s">
         <v>219</v>
       </c>
-      <c r="B113" s="4" t="s">
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
+      <c r="B116" t="s">
         <v>221</v>
       </c>
-      <c r="B114" t="s">
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
+      <c r="B117" t="s">
         <v>223</v>
       </c>
-      <c r="B115" t="s">
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="B118" t="s">
         <v>225</v>
       </c>
-      <c r="B116" t="s">
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+      <c r="B119" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="B117" t="s">
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
+      <c r="B120" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B118" s="4" t="s">
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
+      <c r="B121" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B119" s="4" t="s">
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="B122" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="B120" s="4" t="s">
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+      <c r="B123" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B121" s="4" t="s">
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+      <c r="B124" t="s">
         <v>237</v>
       </c>
-      <c r="B122" s="4" t="s">
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
+      <c r="B125" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>239</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B126" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>241</v>
       </c>
-      <c r="B124" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
+      <c r="B127" t="s">
         <v>242</v>
       </c>
-      <c r="B125" t="s">
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+      <c r="B128" t="s">
         <v>244</v>
-      </c>
-      <c r="B126" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>246</v>
-      </c>
-      <c r="B127" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B37" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B44" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B52" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B60" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B69" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B77" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B86" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B93" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B101" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B110" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B117" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B126" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B29" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B38" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B45" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B53" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B61" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B70" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B78" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B87" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B94" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B102" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B111" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B118" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B127" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updated post default values
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andcolli\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6BBE4B5-E89E-4583-AC0F-097BF4F3A32C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD16B4B-E129-4D2D-BAE7-3D9E73F1A850}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21720" yWindow="-6930" windowWidth="21840" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="249">
   <si>
     <t>FIELDS</t>
   </si>
@@ -768,16 +768,10 @@
     <t>Glasgow Tribunals Centre</t>
   </si>
   <si>
-    <t>3 Atlantic Quay</t>
-  </si>
-  <si>
-    <t>20 York Street</t>
-  </si>
-  <si>
-    <t>tribunalGlasgowAddressLine3</t>
-  </si>
-  <si>
     <t>G2 8GT</t>
+  </si>
+  <si>
+    <t>3 Atlantic Quay, 20 York Street</t>
   </si>
 </sst>
 </file>
@@ -1147,10 +1141,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H128"/>
+  <dimension ref="A1:H127"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,946 +1268,938 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>249</v>
-      </c>
-      <c r="B14" t="s">
-        <v>248</v>
+        <v>24</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>250</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
+        <v>36</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>89</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>107</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="B58" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B60" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>37</v>
+        <v>117</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>122</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="B66" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B68" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B69" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>130</v>
-      </c>
-      <c r="B70" t="s">
-        <v>131</v>
+        <v>132</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>139</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="B75" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B77" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>145</v>
-      </c>
-      <c r="B78" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>152</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>154</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="B83" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B84" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B85" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B86" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>162</v>
-      </c>
-      <c r="B87" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>170</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="B91" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B92" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>176</v>
-      </c>
-      <c r="B94" t="s">
-        <v>177</v>
+        <v>178</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>186</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="B99" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B100" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>192</v>
-      </c>
-      <c r="B102" t="s">
-        <v>193</v>
+        <v>194</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>202</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
+      </c>
+      <c r="B107" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B108" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B109" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B110" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>210</v>
-      </c>
-      <c r="B111" t="s">
-        <v>211</v>
+        <v>212</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>216</v>
-      </c>
-      <c r="B114" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
+      </c>
+      <c r="B114" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B115" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B116" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B117" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>224</v>
-      </c>
-      <c r="B118" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>234</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>235</v>
+        <v>236</v>
+      </c>
+      <c r="B123" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B124" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B125" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B126" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B127" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>243</v>
-      </c>
-      <c r="B128" t="s">
         <v>244</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B29" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B38" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B45" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B53" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B61" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B70" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B78" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B87" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B94" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B102" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B111" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B118" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B127" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B37" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B44" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B52" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B60" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B69" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B77" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B86" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B93" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B101" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B110" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B117" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B126" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Added post default values and tests
</commit_message>
<xml_diff>
--- a/src/main/resources/postDefaultValues.xlsx
+++ b/src/main/resources/postDefaultValues.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://justiceuk-my.sharepoint.com/personal/thomas_hart_justice_gov_uk/Documents/__Project team/ECM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C07C3F0-6108-4B0E-8CFA-53C1669EFD3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{4D5477FF-38BD-4BCA-9F9B-5A328587ED00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FEF91926-40F5-4386-A982-6904DEA472D6}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27912" yWindow="312" windowWidth="23040" windowHeight="13824" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Defaults" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="253">
   <si>
     <t>FIELDS</t>
   </si>
@@ -555,9 +555,6 @@
     <t>tribunalMidlandsEastEmail</t>
   </si>
   <si>
-    <t>e.midlandseastet@justice.gov.uk</t>
-  </si>
-  <si>
     <t>tribunalMidlandsWestAddressLine1</t>
   </si>
   <si>
@@ -693,15 +690,9 @@
     <t>tribunalWalesDX</t>
   </si>
   <si>
-    <t>DX 743942 Caerdydd/Cardiff 38</t>
-  </si>
-  <si>
     <t>tribunalWalesEmail</t>
   </si>
   <si>
-    <t>cardiffet@justice.gov.uk</t>
-  </si>
-  <si>
     <t>tribunalWatfordAddressLine1</t>
   </si>
   <si>
@@ -772,13 +763,34 @@
   </si>
   <si>
     <t>londonsouthet@Justice.gov.uk</t>
+  </si>
+  <si>
+    <t>waleset@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>tribunalWalesAddressLine2</t>
+  </si>
+  <si>
+    <t>tribunalWalesAddressLine3</t>
+  </si>
+  <si>
+    <t>MidlandsEastET@justice.gov.uk</t>
+  </si>
+  <si>
+    <t>317501 Caerdydd/Cardiff 45</t>
+  </si>
+  <si>
+    <t>3rd Floor, Cardiff Magistrates' Court</t>
+  </si>
+  <si>
+    <t>Wales Employment Tribunal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -793,6 +805,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0B0C0C"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -815,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -828,6 +852,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1142,10 +1167,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H127"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,7 +1286,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1269,7 +1294,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1285,7 +1310,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1853,7 +1878,7 @@
         <v>162</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1908,269 +1933,269 @@
       <c r="A93" t="s">
         <v>175</v>
       </c>
-      <c r="B93" t="s">
-        <v>176</v>
+      <c r="B93" s="5" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
+        <v>176</v>
+      </c>
+      <c r="B94" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
+        <v>178</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
+        <v>180</v>
+      </c>
+      <c r="B96" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
+        <v>182</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>183</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
+        <v>184</v>
+      </c>
+      <c r="B98" s="4" t="s">
         <v>185</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
+        <v>186</v>
+      </c>
+      <c r="B99" t="s">
         <v>187</v>
-      </c>
-      <c r="B99" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
+        <v>188</v>
+      </c>
+      <c r="B100" t="s">
         <v>189</v>
-      </c>
-      <c r="B100" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>190</v>
+      </c>
+      <c r="B101" t="s">
         <v>191</v>
-      </c>
-      <c r="B101" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
+        <v>192</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>193</v>
-      </c>
-      <c r="B102" s="4" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
+        <v>194</v>
+      </c>
+      <c r="B103" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
+        <v>196</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>197</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
+        <v>198</v>
+      </c>
+      <c r="B105" s="4" t="s">
         <v>199</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>200</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>201</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>202</v>
+      </c>
+      <c r="B107" t="s">
         <v>203</v>
-      </c>
-      <c r="B107" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
+        <v>204</v>
+      </c>
+      <c r="B108" t="s">
         <v>205</v>
-      </c>
-      <c r="B108" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
+        <v>206</v>
+      </c>
+      <c r="B109" t="s">
         <v>207</v>
-      </c>
-      <c r="B109" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" t="s">
         <v>209</v>
-      </c>
-      <c r="B110" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>212</v>
+        <v>252</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>214</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>215</v>
+        <v>248</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>217</v>
-      </c>
-      <c r="B114" t="s">
-        <v>218</v>
+        <v>212</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>219</v>
-      </c>
-      <c r="B115" t="s">
-        <v>220</v>
+        <v>214</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B116" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B117" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>225</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>226</v>
+        <v>220</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>227</v>
-      </c>
-      <c r="B119" s="4" t="s">
-        <v>228</v>
+        <v>221</v>
+      </c>
+      <c r="B119" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>235</v>
-      </c>
-      <c r="B123" t="s">
-        <v>236</v>
+        <v>228</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>237</v>
-      </c>
-      <c r="B124" t="s">
-        <v>244</v>
+        <v>230</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B125" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B126" t="s">
         <v>241</v>
@@ -2178,13 +2203,30 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="B127" t="s">
-        <v>243</v>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>237</v>
+      </c>
+      <c r="B128" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>239</v>
+      </c>
+      <c r="B129" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B19" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -2195,14 +2237,12 @@
     <hyperlink ref="B60" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="B69" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="B77" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B93" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B101" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="B110" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B117" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="B126" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B101" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B110" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B128" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId15"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2211,6 +2251,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E98ADB2028FC4F43824F86666CC83903" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ff47f26d8558bca2ac2c896a7e751c25">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="bc19a69a-bda7-4614-8881-f2ac618cff8e" xmlns:ns4="02128cc3-8226-4d54-9246-100bb62c9520" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63ef4ea587d9ab0193671c85d2373b1f" ns3:_="" ns4:_="">
     <xsd:import namespace="bc19a69a-bda7-4614-8881-f2ac618cff8e"/>
@@ -2427,22 +2482,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DE8CE9D-6FCC-4918-BBCF-A391DC476C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773F96A2-389E-495E-B90C-F743B326B51C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6DA0F2A6-1E3C-4FCD-B38E-ABBF532BD981}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2459,21 +2516,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773F96A2-389E-495E-B90C-F743B326B51C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DE8CE9D-6FCC-4918-BBCF-A391DC476C60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>